<commit_message>
pulls from directory. multiple string functionality
</commit_message>
<xml_diff>
--- a/xlsx_search/results/search_results.xlsx
+++ b/xlsx_search/results/search_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>JT001_Samples_CM20230607_Foxf1_timecourse.xlsx</t>
+          <t>SAB01_Sample_metasheet.xlsx</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SAB01_Sample_metasheet.xlsx</t>
+          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
+          <t>JT001_Samples_CM20230607_Foxf1_timecourse.xlsx</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -488,138 +488,6 @@
         </is>
       </c>
       <c r="B5" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Sample_metasheet_AE3_Sequencing.xlsx</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
         <is>
           <t>Bulk RNA-seq of human neural differentiation treated with SAG</t>
         </is>

</xml_diff>